<commit_message>
Nuevos tests +  implementación de transformación de imágenes
</commit_message>
<xml_diff>
--- a/TEST/TESTS.xlsx
+++ b/TEST/TESTS.xlsx
@@ -33,9 +33,6 @@
     <style:style style:name="ro1" style:family="table-row">
       <style:table-row-properties style:row-height="0.452cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
     </style:style>
-    <style:style style:name="ro2" style:family="table-row">
-      <style:table-row-properties style:row-height="0.452cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
-    </style:style>
     <style:style style:name="ta1" style:family="table" style:master-page-name="Default">
       <style:table-properties table:display="true" style:writing-mode="lr-tb"/>
     </style:style>
@@ -48,27 +45,17 @@
       <style:paragraph-properties fo:text-align="center" fo:margin-left="0cm"/>
       <style:text-properties fo:color="#b85c00" fo:font-weight="bold" style:font-weight-asian="bold" style:font-weight-complex="bold"/>
     </style:style>
-    <style:style style:name="ce10" style:family="table-cell" style:parent-style-name="Default">
-      <style:table-cell-properties fo:background-color="#fff5ce" style:text-align-source="fix" style:repeat-content="false" fo:border="0.06pt solid #b85c00" style:vertical-align="middle"/>
-      <style:paragraph-properties fo:text-align="center" fo:margin-left="0cm"/>
-      <style:text-properties fo:color="#b85c00" fo:font-weight="bold" style:font-weight-asian="bold" style:font-weight-complex="bold"/>
-    </style:style>
-    <style:style style:name="ce11" style:family="table-cell" style:parent-style-name="Default">
-      <style:table-cell-properties fo:background-color="#fff5ce" style:text-align-source="fix" style:repeat-content="false" fo:border="none" style:vertical-align="middle"/>
-      <style:paragraph-properties fo:text-align="center" fo:margin-left="0cm"/>
-      <style:text-properties fo:color="#666666" style:font-name="Liberation Serif"/>
-    </style:style>
-    <style:style style:name="ce2" style:family="table-cell" style:parent-style-name="Default">
+    <style:style style:name="ce21" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties fo:background-color="#fff5ce" style:text-align-source="fix" style:repeat-content="false" fo:border="none"/>
       <style:paragraph-properties fo:text-align="center" fo:margin-left="0cm"/>
       <style:text-properties fo:color="#666666" style:font-name="Liberation Serif" fo:font-weight="bold" style:font-weight-asian="bold" style:font-weight-complex="bold"/>
     </style:style>
-    <style:style style:name="ce3" style:family="table-cell" style:parent-style-name="Default">
+    <style:style style:name="ce22" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties fo:background-color="#fff5ce" style:text-align-source="fix" style:repeat-content="false" fo:border="0.06pt solid #ffdbb6"/>
       <style:paragraph-properties fo:text-align="center" fo:margin-left="0cm"/>
       <style:text-properties fo:color="#666666" style:font-name="Liberation Serif" fo:font-weight="bold" style:font-weight-asian="bold" style:font-weight-complex="bold"/>
     </style:style>
-    <style:style style:name="ce4" style:family="table-cell" style:parent-style-name="Default">
+    <style:style style:name="ce23" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties fo:background-color="#fff5ce" style:text-align-source="fix" style:repeat-content="false" fo:border="none"/>
       <style:paragraph-properties fo:text-align="center" fo:margin-left="0cm"/>
       <style:text-properties fo:color="#b85c00" fo:font-weight="bold" style:font-weight-asian="bold" style:font-weight-complex="bold"/>
@@ -83,51 +70,6 @@
       <style:paragraph-properties fo:text-align="center" fo:margin-left="0cm"/>
       <style:text-properties fo:color="#666666" style:font-name="Liberation Serif"/>
     </style:style>
-    <style:style style:name="ce7" style:family="table-cell" style:parent-style-name="Default">
-      <style:table-cell-properties fo:background-color="#fff5ce" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="wrap" fo:border="none"/>
-      <style:paragraph-properties fo:text-align="center" fo:margin-left="0cm"/>
-      <style:text-properties fo:color="#666666" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Liberation Serif" fo:font-size="10pt" fo:language="es" fo:country="ES" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:text-underline-mode="continuous" style:text-overline-mode="continuous" style:text-line-through-mode="continuous" style:font-name-asian="Segoe UI" style:font-size-asian="10pt" style:language-asian="zh" style:country-asian="CN" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-name-complex="Tahoma" style:font-size-complex="10pt" style:language-complex="hi" style:country-complex="IN" style:font-style-complex="normal" style:font-weight-complex="normal" style:text-emphasize="none" style:font-relief="none" style:text-overline-style="none" style:text-overline-color="font-color"/>
-    </style:style>
-    <style:style style:name="ce8" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N11">
-      <style:table-cell-properties fo:background-color="#fff5ce" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="wrap" fo:border="none"/>
-      <style:paragraph-properties fo:text-align="center" fo:margin-left="0cm"/>
-      <style:text-properties fo:color="#666666" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Liberation Serif" fo:font-size="10pt" fo:language="es" fo:country="ES" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:text-underline-mode="continuous" style:text-overline-mode="continuous" style:text-line-through-mode="continuous" style:font-name-asian="Segoe UI" style:font-size-asian="10pt" style:language-asian="zh" style:country-asian="CN" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-name-complex="Tahoma" style:font-size-complex="10pt" style:language-complex="hi" style:country-complex="IN" style:font-style-complex="normal" style:font-weight-complex="normal" style:text-emphasize="none" style:font-relief="none" style:text-overline-style="none" style:text-overline-color="font-color"/>
-    </style:style>
-    <style:style style:name="ce9" style:family="table-cell" style:parent-style-name="Default">
-      <style:table-cell-properties fo:background-color="#fff5ce" style:text-align-source="fix" style:repeat-content="false" fo:border="none"/>
-      <style:paragraph-properties fo:text-align="center" fo:margin-left="0cm"/>
-      <style:text-properties fo:color="#666666" style:font-name="Liberation Serif"/>
-    </style:style>
-    <style:style style:name="ce20" style:family="table-cell" style:parent-style-name="Default">
-      <style:table-cell-properties fo:background-color="#fff5ce" style:text-align-source="fix" style:repeat-content="false" fo:border="0.06pt solid #b85c00"/>
-      <style:paragraph-properties fo:text-align="center" fo:margin-left="0cm"/>
-      <style:text-properties fo:color="#b85c00" fo:font-weight="bold" style:font-weight-asian="bold" style:font-weight-complex="bold"/>
-    </style:style>
-    <style:style style:name="ce21" style:family="table-cell" style:parent-style-name="Default">
-      <style:table-cell-properties fo:background-color="#fff5ce" style:text-align-source="fix" style:repeat-content="false" fo:border="none"/>
-      <style:paragraph-properties fo:text-align="center" fo:margin-left="0cm"/>
-      <style:text-properties fo:color="#666666" style:font-name="Liberation Serif" fo:font-weight="bold" style:font-weight-asian="bold" style:font-weight-complex="bold"/>
-    </style:style>
-    <style:style style:name="ce22" style:family="table-cell" style:parent-style-name="Default">
-      <style:table-cell-properties fo:background-color="#fff5ce" style:text-align-source="fix" style:repeat-content="false" fo:border="0.06pt solid #ffdbb6"/>
-      <style:paragraph-properties fo:text-align="center" fo:margin-left="0cm"/>
-      <style:text-properties fo:color="#666666" style:font-name="Liberation Serif" fo:font-weight="bold" style:font-weight-asian="bold" style:font-weight-complex="bold"/>
-    </style:style>
-    <style:style style:name="ce23" style:family="table-cell" style:parent-style-name="Default">
-      <style:table-cell-properties fo:background-color="#fff5ce" style:text-align-source="fix" style:repeat-content="false" fo:border="none"/>
-      <style:paragraph-properties fo:text-align="center" fo:margin-left="0cm"/>
-      <style:text-properties fo:color="#b85c00" fo:font-weight="bold" style:font-weight-asian="bold" style:font-weight-complex="bold"/>
-    </style:style>
-    <style:style style:name="ce24" style:family="table-cell" style:parent-style-name="Default">
-      <style:table-cell-properties fo:background-color="#fff5ce" style:text-align-source="fix" style:repeat-content="false" fo:border="0.06pt solid #ffdbb6" style:vertical-align="middle"/>
-      <style:paragraph-properties fo:text-align="center" fo:margin-left="0cm"/>
-      <style:text-properties fo:color="#666666" style:font-name="Liberation Serif"/>
-    </style:style>
-    <style:style style:name="ce25" style:family="table-cell" style:parent-style-name="Default">
-      <style:table-cell-properties fo:background-color="#fff5ce" style:text-align-source="fix" style:repeat-content="false" fo:border="0.06pt solid #ffdbb6"/>
-      <style:paragraph-properties fo:text-align="center" fo:margin-left="0cm"/>
-      <style:text-properties fo:color="#666666" style:font-name="Liberation Serif"/>
-    </style:style>
     <style:style style:name="ce26" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties fo:background-color="#fff5ce" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="wrap" fo:border="none"/>
       <style:paragraph-properties fo:text-align="center" fo:margin-left="0cm"/>
@@ -137,6 +79,11 @@
       <style:table-cell-properties fo:background-color="#fff5ce" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="wrap" fo:border="none"/>
       <style:paragraph-properties fo:text-align="center" fo:margin-left="0cm"/>
       <style:text-properties fo:color="#666666" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Liberation Serif" fo:font-size="10pt" fo:language="es" fo:country="ES" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:text-underline-mode="continuous" style:text-overline-mode="continuous" style:text-line-through-mode="continuous" style:font-name-asian="Segoe UI" style:font-size-asian="10pt" style:language-asian="zh" style:country-asian="CN" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-name-complex="Tahoma" style:font-size-complex="10pt" style:language-complex="hi" style:country-complex="IN" style:font-style-complex="normal" style:font-weight-complex="normal" style:text-emphasize="none" style:font-relief="none" style:text-overline-style="none" style:text-overline-color="font-color"/>
+    </style:style>
+    <style:style style:name="ce9" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N11">
+      <style:table-cell-properties fo:background-color="#fff5ce" style:text-align-source="fix" style:repeat-content="false" fo:border="0.06pt solid #ffdbb6"/>
+      <style:paragraph-properties fo:text-align="center" fo:margin-left="0cm"/>
+      <style:text-properties fo:color="#666666" style:font-name="Liberation Serif"/>
     </style:style>
     <style:style style:name="ce28" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties fo:background-color="#fff5ce" style:text-align-source="fix" style:repeat-content="false" fo:border="none"/>
@@ -159,50 +106,50 @@
       <table:calculation-settings table:automatic-find-labels="false" table:use-regular-expressions="false" table:use-wildcards="true"/>
       <table:table table:name="Hoja1" table:style-name="ta1">
         <table:table-column table:style-name="co1" table:default-cell-style-name="ce22"/>
-        <table:table-column table:style-name="co1" table:number-columns-repeated="8" table:default-cell-style-name="ce25"/>
-        <table:table-column table:style-name="co2" table:default-cell-style-name="ce25"/>
-        <table:table-column table:style-name="co1" table:default-cell-style-name="ce24"/>
-        <table:table-column table:style-name="co1" table:number-columns-repeated="2" table:default-cell-style-name="ce25"/>
+        <table:table-column table:style-name="co1" table:number-columns-repeated="8" table:default-cell-style-name="ce6"/>
+        <table:table-column table:style-name="co2" table:default-cell-style-name="ce6"/>
+        <table:table-column table:style-name="co1" table:default-cell-style-name="ce5"/>
+        <table:table-column table:style-name="co1" table:number-columns-repeated="2" table:default-cell-style-name="ce6"/>
         <table:table-row table:style-name="ro1" table:number-rows-repeated="2">
           <table:table-cell table:style-name="Default" table:number-columns-repeated="13"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
-          <table:table-cell table:style-name="ce20" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
             <text:p>TEST</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce23"/>
-          <table:table-cell table:style-name="ce20" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
             <text:p>NETWORK</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce20" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
             <text:p>ACCURACY</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce20" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
             <text:p>DEVIATION</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce23"/>
-          <table:table-cell table:style-name="ce20" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
             <text:p>FOLDS</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce20" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
             <text:p>EPOCHS</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce20" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
             <text:p>LR</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce20" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
             <text:p>MOMENTUM</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce29" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="3" table:number-rows-spanned="1">
             <text:p>OTHER REQUERIMENTS</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce20"/>
+          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce1"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell table:style-name="ce21" office:value-type="float" office:value="1" calcext:value-type="float">
             <text:p>1</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce24" table:number-columns-spanned="1" table:number-rows-spanned="50"/>
+          <table:table-cell table:style-name="ce5" table:number-columns-spanned="1" table:number-rows-spanned="50"/>
           <table:table-cell table:style-name="ce26" office:value-type="string" calcext:value-type="string">
             <text:p>NN04 </text:p>
           </table:table-cell>
@@ -212,7 +159,7 @@
           <table:table-cell table:style-name="ce27" office:value-type="percentage" office:value="0.152008922106566" calcext:value-type="percentage">
             <text:p>15,20 %</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce24" table:number-columns-spanned="1" table:number-rows-spanned="50"/>
+          <table:table-cell table:style-name="ce5" table:number-columns-spanned="1" table:number-rows-spanned="50"/>
           <table:table-cell table:style-name="ce28" office:value-type="float" office:value="10" calcext:value-type="float">
             <text:p>10</text:p>
           </table:table-cell>
@@ -233,9 +180,31 @@
             <text:p>2</text:p>
           </table:table-cell>
           <table:covered-table-cell/>
-          <table:table-cell table:number-columns-repeated="3"/>
-          <table:covered-table-cell/>
-          <table:table-cell table:number-columns-repeated="4"/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>NN01</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce9" office:value-type="percentage" office:value="0.663" calcext:value-type="percentage">
+            <text:p>66,30 %</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce9" office:value-type="percentage" office:value="0.107738720987396" calcext:value-type="percentage">
+            <text:p>10,77 %</text:p>
+          </table:table-cell>
+          <table:covered-table-cell/>
+          <table:table-cell office:value-type="float" office:value="10" calcext:value-type="float">
+            <text:p>10</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="15" calcext:value-type="float">
+            <text:p>15</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="0.01" calcext:value-type="float">
+            <text:p>0,01</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:s/>
+              - 
+            </text:p>
+          </table:table-cell>
           <table:table-cell table:number-columns-spanned="3" table:number-rows-spanned="1"/>
           <table:covered-table-cell table:number-columns-repeated="2"/>
         </table:table-row>
@@ -244,10 +213,37 @@
             <text:p>3</text:p>
           </table:table-cell>
           <table:covered-table-cell/>
-          <table:table-cell table:number-columns-repeated="3"/>
-          <table:covered-table-cell/>
-          <table:table-cell table:number-columns-repeated="4"/>
-          <table:table-cell table:number-columns-spanned="3" table:number-rows-spanned="1"/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>NN02</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce9" office:value-type="percentage" office:value="0.6702" calcext:value-type="percentage">
+            <text:p>67,02 %</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce9" office:value-type="percentage" office:value="0.010891" calcext:value-type="percentage">
+            <text:p>1,09 %</text:p>
+          </table:table-cell>
+          <table:covered-table-cell/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:s/>
+              - 
+            </text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="100" calcext:value-type="float">
+            <text:p>100</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="0.01" calcext:value-type="float">
+            <text:p>0,01</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:s/>
+              - 
+            </text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string" table:number-columns-spanned="3" table:number-rows-spanned="1">
+            <text:p>TransformConfig</text:p>
+          </table:table-cell>
           <table:covered-table-cell table:number-columns-repeated="2"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
@@ -255,10 +251,34 @@
             <text:p>4</text:p>
           </table:table-cell>
           <table:covered-table-cell/>
-          <table:table-cell table:number-columns-repeated="3"/>
-          <table:covered-table-cell/>
-          <table:table-cell table:number-columns-repeated="4"/>
-          <table:table-cell table:number-columns-spanned="3" table:number-rows-spanned="1"/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>NN02</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce9" office:value-type="percentage" office:value="0.71952" calcext:value-type="percentage">
+            <text:p>71,95 %</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce9" office:value-type="percentage" office:value="0.0488905062358737" calcext:value-type="percentage">
+            <text:p>4,89 %</text:p>
+          </table:table-cell>
+          <table:covered-table-cell/>
+          <table:table-cell office:value-type="float" office:value="10" calcext:value-type="float">
+            <text:p>10</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="0.01" calcext:value-type="float">
+            <text:p>0,01</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:s/>
+              - 
+            </text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string" table:number-columns-spanned="3" table:number-rows-spanned="1">
+            <text:p>TransformConfig, batch_size=100</text:p>
+          </table:table-cell>
           <table:covered-table-cell table:number-columns-repeated="2"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
@@ -778,11 +798,11 @@
 <office:document-meta xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" office:version="1.3">
   <office:meta>
     <meta:creation-date>2024-05-15T15:56:32.968000000</meta:creation-date>
-    <dc:date>2024-05-15T16:34:52.098000000</dc:date>
-    <meta:editing-duration>PT7M47S</meta:editing-duration>
-    <meta:editing-cycles>4</meta:editing-cycles>
+    <dc:date>2024-05-21T21:27:26.527000000</dc:date>
+    <meta:editing-duration>PT3H4M34S</meta:editing-duration>
+    <meta:editing-cycles>5</meta:editing-cycles>
     <meta:generator>LibreOffice/7.1.0.3$Windows_X86_64 LibreOffice_project/f6099ecf3d29644b5008cc8f48f42f4a40986e4c</meta:generator>
-    <meta:document-statistic meta:table-count="1" meta:cell-count="66" meta:object-count="0"/>
+    <meta:document-statistic meta:table-count="1" meta:cell-count="89" meta:object-count="0"/>
   </office:meta>
 </office:document-meta>
 </file>
@@ -800,8 +820,8 @@
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Hoja1">
-              <config:config-item config:name="CursorPositionX" config:type="int">3</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">14</config:config-item>
+              <config:config-item config:name="CursorPositionX" config:type="int">9</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">9</config:config-item>
               <config:config-item config:name="HorizontalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="VerticalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="HorizontalSplitPosition" config:type="int">0</config:config-item>
@@ -1032,9 +1052,9 @@
         </style:region-left>
         <style:region-right>
           <text:p>
-            <text:date style:data-style-name="N2" text:date-value="2024-05-15">00/00/0000</text:date>
+            <text:date style:data-style-name="N2" text:date-value="2024-05-21">00/00/0000</text:date>
             , 
-            <text:time style:data-style-name="N2" text:time-value="16:35:59.166000000">00:00:00</text:time>
+            <text:time style:data-style-name="N2" text:time-value="16:39:27.512000000">00:00:00</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>